<commit_message>
completed the project without multiplication
</commit_message>
<xml_diff>
--- a/Datasheet-main.xlsx
+++ b/Datasheet-main.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CourseUni\2021_Fall\CSE332.10\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89676B54-5757-4264-8715-63765552B509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389FC6EE-080C-44F3-8D96-9CED3E04B2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{EFC6CC18-B430-45A3-AE92-BF6C5C99D8E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EFC6CC18-B430-45A3-AE92-BF6C5C99D8E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>ALUOp</t>
   </si>
@@ -78,13 +77,121 @@
   </si>
   <si>
     <t>XOR</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS</t>
+  </si>
+  <si>
+    <t>OPCODE</t>
+  </si>
+  <si>
+    <t>Reg.Dst</t>
+  </si>
+  <si>
+    <t>Write En</t>
+  </si>
+  <si>
+    <t>ALUSrc</t>
+  </si>
+  <si>
+    <t>Alu Op 1</t>
+  </si>
+  <si>
+    <t>ALU Op 0</t>
+  </si>
+  <si>
+    <t>C.in</t>
+  </si>
+  <si>
+    <t>lw</t>
+  </si>
+  <si>
+    <t>sw</t>
+  </si>
+  <si>
+    <t>MemToReg</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>SLL_SRL</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>LW</t>
+  </si>
+  <si>
+    <t>ADDi</t>
+  </si>
+  <si>
+    <t>Ori</t>
+  </si>
+  <si>
+    <t>SUBi</t>
+  </si>
+  <si>
+    <t>XORi</t>
+  </si>
+  <si>
+    <t>SLL</t>
+  </si>
+  <si>
+    <t>SRL</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>0010</t>
+  </si>
+  <si>
+    <t>0011</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>0110</t>
+  </si>
+  <si>
+    <t>0111</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>CONTROL UNIT TRUTH TABLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,16 +199,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,13 +236,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,80 +586,756 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EF6E5B-A7A6-4ABA-9B02-8A94EFD89460}">
-  <dimension ref="B7:E13"/>
+  <dimension ref="B5:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="17" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" style="1" customWidth="1"/>
+    <col min="15" max="18" width="9.140625" style="1"/>
+    <col min="19" max="19" width="13.85546875" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="L5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="H7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="H8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>0</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0</v>
+      </c>
+      <c r="S8" s="4">
+        <v>0</v>
+      </c>
+      <c r="T8" s="4">
+        <v>0</v>
+      </c>
+      <c r="U8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="1" t="s">
+      <c r="H9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0</v>
+      </c>
+      <c r="T9" s="4">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="H10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>0</v>
+      </c>
+      <c r="R10" s="4">
+        <v>0</v>
+      </c>
+      <c r="S10" s="4">
+        <v>0</v>
+      </c>
+      <c r="T10" s="4">
+        <v>0</v>
+      </c>
+      <c r="U10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
+      <c r="H11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>1</v>
+      </c>
+      <c r="P11" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>0</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0</v>
+      </c>
+      <c r="S11" s="4">
+        <v>0</v>
+      </c>
+      <c r="T11" s="4">
+        <v>0</v>
+      </c>
+      <c r="U11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+      <c r="H12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0</v>
+      </c>
+      <c r="P12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>0</v>
+      </c>
+      <c r="R12" s="4">
+        <v>0</v>
+      </c>
+      <c r="S12" s="4">
+        <v>0</v>
+      </c>
+      <c r="T12" s="4">
+        <v>0</v>
+      </c>
+      <c r="U12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>1</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>0</v>
+      </c>
+      <c r="R13" s="4">
+        <v>1</v>
+      </c>
+      <c r="S13" s="4">
+        <v>0</v>
+      </c>
+      <c r="T13" s="4">
+        <v>0</v>
+      </c>
+      <c r="U13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>1</v>
+      </c>
+      <c r="R14" s="4">
+        <v>0</v>
+      </c>
+      <c r="S14" s="4">
+        <v>1</v>
+      </c>
+      <c r="T14" s="4">
+        <v>0</v>
+      </c>
+      <c r="U14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>0</v>
+      </c>
+      <c r="R15" s="4">
+        <v>0</v>
+      </c>
+      <c r="S15" s="4">
+        <v>0</v>
+      </c>
+      <c r="T15" s="4">
+        <v>0</v>
+      </c>
+      <c r="U15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="H16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="4">
+        <v>1</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>1</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>0</v>
+      </c>
+      <c r="R16" s="4">
+        <v>0</v>
+      </c>
+      <c r="S16" s="4">
+        <v>0</v>
+      </c>
+      <c r="T16" s="4">
+        <v>0</v>
+      </c>
+      <c r="U16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="4">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
+        <v>1</v>
+      </c>
+      <c r="L17" s="4">
+        <v>1</v>
+      </c>
+      <c r="M17" s="4">
+        <v>1</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0</v>
+      </c>
+      <c r="P17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>0</v>
+      </c>
+      <c r="R17" s="4">
+        <v>0</v>
+      </c>
+      <c r="S17" s="4">
+        <v>0</v>
+      </c>
+      <c r="T17" s="4">
+        <v>0</v>
+      </c>
+      <c r="U17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="4">
+        <v>1</v>
+      </c>
+      <c r="K18" s="4">
+        <v>1</v>
+      </c>
+      <c r="L18" s="4">
+        <v>1</v>
+      </c>
+      <c r="M18" s="4">
+        <v>1</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <v>1</v>
+      </c>
+      <c r="P18" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4">
+        <v>0</v>
+      </c>
+      <c r="S18" s="4">
+        <v>0</v>
+      </c>
+      <c r="T18" s="4">
+        <v>0</v>
+      </c>
+      <c r="U18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="4">
+        <v>1</v>
+      </c>
+      <c r="K19" s="4">
+        <v>1</v>
+      </c>
+      <c r="L19" s="4">
+        <v>1</v>
+      </c>
+      <c r="M19" s="4">
+        <v>1</v>
+      </c>
+      <c r="N19" s="4">
+        <v>1</v>
+      </c>
+      <c r="O19" s="4">
+        <v>0</v>
+      </c>
+      <c r="P19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>0</v>
+      </c>
+      <c r="R19" s="4">
+        <v>0</v>
+      </c>
+      <c r="S19" s="4">
+        <v>0</v>
+      </c>
+      <c r="T19" s="4">
+        <v>0</v>
+      </c>
+      <c r="U19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1</v>
+      </c>
+      <c r="K20" s="4">
+        <v>1</v>
+      </c>
+      <c r="L20" s="4">
+        <v>1</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0</v>
+      </c>
+      <c r="O20" s="4">
+        <v>0</v>
+      </c>
+      <c r="P20" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>0</v>
+      </c>
+      <c r="R20" s="4">
+        <v>0</v>
+      </c>
+      <c r="S20" s="4">
+        <v>0</v>
+      </c>
+      <c r="T20" s="4">
+        <v>1</v>
+      </c>
+      <c r="U20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1</v>
+      </c>
+      <c r="L21" s="4">
+        <v>1</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0</v>
+      </c>
+      <c r="O21" s="4">
+        <v>0</v>
+      </c>
+      <c r="P21" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>0</v>
+      </c>
+      <c r="R21" s="4">
+        <v>0</v>
+      </c>
+      <c r="S21" s="4">
+        <v>0</v>
+      </c>
+      <c r="T21" s="4">
+        <v>1</v>
+      </c>
+      <c r="U21" s="4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>